<commit_message>
Move script files of IISBMP1 to dropbox, start working on IISBMP1 until clean.R
</commit_message>
<xml_diff>
--- a/experiments/IISBMP1/data/biogas_and_setup.xlsx
+++ b/experiments/IISBMP1/data/biogas_and_setup.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Documents\GitHub\GD-BMP\experiments\IISBMP1\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au521230\Documents\GitHub\GD-BMP\experiments\IISBMP1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0163AE09-A485-481C-BAE3-DB35BEE3D178}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="992" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="992" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
     <sheet name="VPM" sheetId="2" r:id="rId2"/>
     <sheet name="ChangeLog" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,12 +32,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
   </authors>
   <commentList>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -739,7 +738,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -1355,7 +1354,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMI45"/>
   <sheetViews>
     <sheetView windowProtection="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
@@ -4050,14 +4049,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J421"/>
   <sheetViews>
-    <sheetView windowProtection="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B402" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A320" sqref="A320"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16526,10 +16525,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" workbookViewId="0">
+    <sheetView windowProtection="1" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix typo in data and add new yld plot for appendix
</commit_message>
<xml_diff>
--- a/experiments/IISBMP1/data/biogas_and_setup.xlsx
+++ b/experiments/IISBMP1/data/biogas_and_setup.xlsx
@@ -10,13 +10,16 @@
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="992" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="8190" tabRatio="992" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" r:id="rId1"/>
     <sheet name="Biogas" sheetId="4" r:id="rId2"/>
     <sheet name="ChangeLog" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Biogas!$A$1:$K$421</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3960,10 +3963,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K421"/>
   <sheetViews>
-    <sheetView windowProtection="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F423" sqref="F423"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4016,7 +4020,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
         <v>18</v>
       </c>
@@ -4051,7 +4055,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -4083,7 +4087,7 @@
         <v>1036.5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20">
         <v>1</v>
       </c>
@@ -4115,7 +4119,7 @@
         <v>1032.2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20">
         <v>1</v>
       </c>
@@ -4147,7 +4151,7 @@
         <v>1078.3</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="20">
         <v>1</v>
       </c>
@@ -4179,7 +4183,7 @@
         <v>1046.8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20">
         <v>1</v>
       </c>
@@ -4211,7 +4215,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="20">
         <v>1</v>
       </c>
@@ -4243,7 +4247,7 @@
         <v>1028.5999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20">
         <v>1</v>
       </c>
@@ -4275,7 +4279,7 @@
         <v>1054.5999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20">
         <v>1</v>
       </c>
@@ -4307,7 +4311,7 @@
         <v>1023.9</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20">
         <v>1</v>
       </c>
@@ -4339,7 +4343,7 @@
         <v>1037.9000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20">
         <v>1</v>
       </c>
@@ -4371,7 +4375,7 @@
         <v>1057.5999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20">
         <v>1</v>
       </c>
@@ -4403,7 +4407,7 @@
         <v>1065.9000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20">
         <v>1</v>
       </c>
@@ -4435,7 +4439,7 @@
         <v>1055.9000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20">
         <v>1</v>
       </c>
@@ -4467,7 +4471,7 @@
         <v>1045.5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20">
         <v>1</v>
       </c>
@@ -4499,7 +4503,7 @@
         <v>1058.7</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20">
         <v>1</v>
       </c>
@@ -4531,7 +4535,7 @@
         <v>1036.4000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20">
         <v>1</v>
       </c>
@@ -4563,7 +4567,7 @@
         <v>1052.5999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20">
         <v>1</v>
       </c>
@@ -4595,7 +4599,7 @@
         <v>1029.9000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20">
         <v>1</v>
       </c>
@@ -4627,7 +4631,7 @@
         <v>1025.2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20">
         <v>1</v>
       </c>
@@ -4659,7 +4663,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="20">
         <v>1</v>
       </c>
@@ -4691,7 +4695,7 @@
         <v>1073.5999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="20">
         <v>1</v>
       </c>
@@ -4723,7 +4727,7 @@
         <v>1057.7</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20">
         <v>1</v>
       </c>
@@ -4755,7 +4759,7 @@
         <v>1035.4000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20">
         <v>1</v>
       </c>
@@ -4787,7 +4791,7 @@
         <v>1051.5999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20">
         <v>1</v>
       </c>
@@ -4819,7 +4823,7 @@
         <v>1065.5999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="20">
         <v>1</v>
       </c>
@@ -4849,7 +4853,7 @@
         <v>1055.5999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="20">
         <v>1</v>
       </c>
@@ -4884,7 +4888,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20">
         <v>1</v>
       </c>
@@ -4914,7 +4918,7 @@
         <v>1023.2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="20">
         <v>1</v>
       </c>
@@ -4946,7 +4950,7 @@
         <v>1037.3</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="20">
         <v>1</v>
       </c>
@@ -4978,7 +4982,7 @@
         <v>1057.0999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="20">
         <v>1</v>
       </c>
@@ -5008,7 +5012,7 @@
         <v>1028.4000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="20">
         <v>1</v>
       </c>
@@ -5043,7 +5047,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="20">
         <v>1</v>
       </c>
@@ -5075,7 +5079,7 @@
         <v>1037.5</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="20">
         <v>1</v>
       </c>
@@ -5107,7 +5111,7 @@
         <v>1037.8</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="20">
         <v>1</v>
       </c>
@@ -5139,7 +5143,7 @@
         <v>1028.5</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="20">
         <v>1</v>
       </c>
@@ -5174,7 +5178,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="20">
         <v>1</v>
       </c>
@@ -5206,7 +5210,7 @@
         <v>1036.3</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="20">
         <v>1</v>
       </c>
@@ -5238,7 +5242,7 @@
         <v>1032.0999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="20">
         <v>1</v>
       </c>
@@ -5270,7 +5274,7 @@
         <v>1078.2</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="20">
         <v>1</v>
       </c>
@@ -5302,7 +5306,7 @@
         <v>1046.5999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="20">
         <v>1</v>
       </c>
@@ -5325,7 +5329,7 @@
         <v>1073.5999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="20">
         <v>1</v>
       </c>
@@ -5357,7 +5361,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="20">
         <v>1</v>
       </c>
@@ -5389,7 +5393,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="20">
         <v>1</v>
       </c>
@@ -5418,7 +5422,7 @@
         <v>1049.9000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="20">
         <v>1</v>
       </c>
@@ -5444,7 +5448,7 @@
         <v>1035.9000000000001</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="20">
         <v>1</v>
       </c>
@@ -5476,7 +5480,7 @@
         <v>1022.6</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="20">
         <v>1</v>
       </c>
@@ -5508,7 +5512,7 @@
         <v>1036.5999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="20">
         <v>1</v>
       </c>
@@ -5540,7 +5544,7 @@
         <v>1056.5</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="20">
         <v>1</v>
       </c>
@@ -5572,7 +5576,7 @@
         <v>1065.0999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="20">
         <v>1</v>
       </c>
@@ -5604,7 +5608,7 @@
         <v>1055.0999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="20">
         <v>1</v>
       </c>
@@ -5639,7 +5643,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="20">
         <v>1</v>
       </c>
@@ -5671,7 +5675,7 @@
         <v>1037.4000000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="20">
         <v>1</v>
       </c>
@@ -5703,7 +5707,7 @@
         <v>1027.9000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="20">
         <v>1</v>
       </c>
@@ -5735,7 +5739,7 @@
         <v>1053.9000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="20">
         <v>1</v>
       </c>
@@ -5767,7 +5771,7 @@
         <v>1036.2</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="20">
         <v>1</v>
       </c>
@@ -5799,7 +5803,7 @@
         <v>1032.0999999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="20">
         <v>1</v>
       </c>
@@ -5831,7 +5835,7 @@
         <v>1078.2</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="20">
         <v>1</v>
       </c>
@@ -5866,7 +5870,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="20">
         <v>1</v>
       </c>
@@ -5889,7 +5893,7 @@
         <v>1073.8</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="20">
         <v>1</v>
       </c>
@@ -5921,7 +5925,7 @@
         <v>1035.7</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="20">
         <v>1</v>
       </c>
@@ -5953,7 +5957,7 @@
         <v>1055.5</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="20">
         <v>1</v>
       </c>
@@ -5985,7 +5989,7 @@
         <v>1033.3</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="20">
         <v>1</v>
       </c>
@@ -6017,7 +6021,7 @@
         <v>1049.4000000000001</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="20">
         <v>1</v>
       </c>
@@ -6049,7 +6053,7 @@
         <v>1035.0999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="20">
         <v>1</v>
       </c>
@@ -6081,7 +6085,7 @@
         <v>1064.0999999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="20">
         <v>1</v>
       </c>
@@ -6113,7 +6117,7 @@
         <v>1054.0999999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="20">
         <v>1</v>
       </c>
@@ -6145,7 +6149,7 @@
         <v>1043.7</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="20">
         <v>1</v>
       </c>
@@ -6177,7 +6181,7 @@
         <v>1036.5</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="20">
         <v>1</v>
       </c>
@@ -6209,7 +6213,7 @@
         <v>1027.2</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="20">
         <v>1</v>
       </c>
@@ -6241,7 +6245,7 @@
         <v>1053.3</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="20">
         <v>1</v>
       </c>
@@ -6273,7 +6277,7 @@
         <v>1022.1</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="20">
         <v>1</v>
       </c>
@@ -6305,7 +6309,7 @@
         <v>1036.2</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="20">
         <v>1</v>
       </c>
@@ -6337,7 +6341,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="20">
         <v>1</v>
       </c>
@@ -6363,7 +6367,7 @@
         <v>0.60499999999999998</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="20">
         <v>1</v>
       </c>
@@ -6386,7 +6390,7 @@
         <v>1073.5999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="20">
         <v>1</v>
       </c>
@@ -6418,7 +6422,7 @@
         <v>1036.0999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="20">
         <v>1</v>
       </c>
@@ -6450,7 +6454,7 @@
         <v>1026.8</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="20">
         <v>1</v>
       </c>
@@ -6482,7 +6486,7 @@
         <v>1052.8</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="20">
         <v>1</v>
       </c>
@@ -6514,7 +6518,7 @@
         <v>1063.3</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="20">
         <v>1</v>
       </c>
@@ -6546,7 +6550,7 @@
         <v>1053</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="20">
         <v>1</v>
       </c>
@@ -6578,7 +6582,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="20">
         <v>1</v>
       </c>
@@ -6610,7 +6614,7 @@
         <v>1021.8</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="20">
         <v>1</v>
       </c>
@@ -6642,7 +6646,7 @@
         <v>1035.9000000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="20">
         <v>1</v>
       </c>
@@ -6674,7 +6678,7 @@
         <v>1055.7</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="20">
         <v>1</v>
       </c>
@@ -6706,7 +6710,7 @@
         <v>1055.0999999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="20">
         <v>1</v>
       </c>
@@ -6738,7 +6742,7 @@
         <v>1032.8</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="20">
         <v>1</v>
       </c>
@@ -6770,7 +6774,7 @@
         <v>1048.9000000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="20">
         <v>1</v>
       </c>
@@ -6802,7 +6806,7 @@
         <v>1036.0999999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="20">
         <v>1</v>
       </c>
@@ -6834,7 +6838,7 @@
         <v>1031.8</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="20">
         <v>1</v>
       </c>
@@ -6866,7 +6870,7 @@
         <v>1077.9000000000001</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="20">
         <v>1</v>
       </c>
@@ -6898,7 +6902,7 @@
         <v>1046.4000000000001</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="20">
         <v>1</v>
       </c>
@@ -6930,7 +6934,7 @@
         <v>1034.7</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="20">
         <v>1</v>
       </c>
@@ -6962,7 +6966,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="20">
         <v>1</v>
       </c>
@@ -6994,7 +6998,7 @@
         <v>1031.7</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="20">
         <v>1</v>
       </c>
@@ -7026,7 +7030,7 @@
         <v>1077.8</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="20">
         <v>1</v>
       </c>
@@ -7058,7 +7062,7 @@
         <v>1046.3</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="20">
         <v>1</v>
       </c>
@@ -7090,7 +7094,7 @@
         <v>1054.7</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="20">
         <v>1</v>
       </c>
@@ -7122,7 +7126,7 @@
         <v>1032.5</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="20">
         <v>1</v>
       </c>
@@ -7154,7 +7158,7 @@
         <v>1048.5</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="20">
         <v>1</v>
       </c>
@@ -7186,7 +7190,7 @@
         <v>1034.4000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="20">
         <v>1</v>
       </c>
@@ -7218,7 +7222,7 @@
         <v>1063.2</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="20">
         <v>1</v>
       </c>
@@ -7250,7 +7254,7 @@
         <v>1052.5999999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="20">
         <v>1</v>
       </c>
@@ -7282,7 +7286,7 @@
         <v>1042.8</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="20">
         <v>1</v>
       </c>
@@ -7314,7 +7318,7 @@
         <v>1021.5</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="20">
         <v>1</v>
       </c>
@@ -7346,7 +7350,7 @@
         <v>1035.5999999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="20">
         <v>1</v>
       </c>
@@ -7378,7 +7382,7 @@
         <v>1055.4000000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="20">
         <v>1</v>
       </c>
@@ -7410,7 +7414,7 @@
         <v>1035.7</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="20">
         <v>1</v>
       </c>
@@ -7442,7 +7446,7 @@
         <v>1026.4000000000001</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="20">
         <v>1</v>
       </c>
@@ -7474,7 +7478,7 @@
         <v>1052.4000000000001</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="20">
         <v>1</v>
       </c>
@@ -7497,7 +7501,7 @@
         <v>1073.5999999999999</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="20">
         <v>1</v>
       </c>
@@ -7520,7 +7524,7 @@
         <v>1073.5999999999999</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="20">
         <v>1</v>
       </c>
@@ -7552,7 +7556,7 @@
         <v>1021.2</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="20">
         <v>1</v>
       </c>
@@ -7584,7 +7588,7 @@
         <v>1035.3</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="20">
         <v>1</v>
       </c>
@@ -7616,7 +7620,7 @@
         <v>1055.0999999999999</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="20">
         <v>1</v>
       </c>
@@ -7648,7 +7652,7 @@
         <v>1035.4000000000001</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="20">
         <v>1</v>
       </c>
@@ -7680,7 +7684,7 @@
         <v>1026.0999999999999</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="20">
         <v>1</v>
       </c>
@@ -7712,7 +7716,7 @@
         <v>1052.0999999999999</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="20">
         <v>1</v>
       </c>
@@ -7744,7 +7748,7 @@
         <v>1054.3</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="20">
         <v>1</v>
       </c>
@@ -7776,7 +7780,7 @@
         <v>1032.0999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="20">
         <v>1</v>
       </c>
@@ -7808,7 +7812,7 @@
         <v>1048.0999999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="20">
         <v>1</v>
       </c>
@@ -7843,7 +7847,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="20">
         <v>1</v>
       </c>
@@ -7875,7 +7879,7 @@
         <v>1052.5999999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="20">
         <v>1</v>
       </c>
@@ -7907,7 +7911,7 @@
         <v>1042.5999999999999</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="20">
         <v>1</v>
       </c>
@@ -7939,7 +7943,7 @@
         <v>1035.8</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="20">
         <v>1</v>
       </c>
@@ -7971,7 +7975,7 @@
         <v>1031.5999999999999</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="20">
         <v>1</v>
       </c>
@@ -8003,7 +8007,7 @@
         <v>1077.5999999999999</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="20">
         <v>1</v>
       </c>
@@ -8035,7 +8039,7 @@
         <v>1046.2</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="20">
         <v>1</v>
       </c>
@@ -8070,7 +8074,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="20">
         <v>1</v>
       </c>
@@ -8102,7 +8106,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="20">
         <v>1</v>
       </c>
@@ -8134,7 +8138,7 @@
         <v>1035.0999999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="20">
         <v>1</v>
       </c>
@@ -8166,7 +8170,7 @@
         <v>1054.9000000000001</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="20">
         <v>1</v>
       </c>
@@ -8198,7 +8202,7 @@
         <v>1035.0999999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="20">
         <v>1</v>
       </c>
@@ -8230,7 +8234,7 @@
         <v>1025.9000000000001</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="20">
         <v>1</v>
       </c>
@@ -8262,7 +8266,7 @@
         <v>1051.8</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="20">
         <v>1</v>
       </c>
@@ -8294,7 +8298,7 @@
         <v>1054</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="20">
         <v>1</v>
       </c>
@@ -8326,7 +8330,7 @@
         <v>1031.9000000000001</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="20">
         <v>1</v>
       </c>
@@ -8358,7 +8362,7 @@
         <v>1047.9000000000001</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="20">
         <v>1</v>
       </c>
@@ -8390,7 +8394,7 @@
         <v>1062.9000000000001</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="20">
         <v>1</v>
       </c>
@@ -8422,7 +8426,7 @@
         <v>1052.5</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="20">
         <v>1</v>
       </c>
@@ -8454,7 +8458,7 @@
         <v>1042.5</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="20">
         <v>1</v>
       </c>
@@ -8486,7 +8490,7 @@
         <v>1035.7</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="20">
         <v>1</v>
       </c>
@@ -8518,7 +8522,7 @@
         <v>1031.4000000000001</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="20">
         <v>1</v>
       </c>
@@ -8550,7 +8554,7 @@
         <v>1077.5</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="20">
         <v>1</v>
       </c>
@@ -8582,7 +8586,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="20">
         <v>1</v>
       </c>
@@ -8614,7 +8618,7 @@
         <v>1033.9000000000001</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="20">
         <v>1</v>
       </c>
@@ -8637,7 +8641,7 @@
         <v>1073.5999999999999</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="20">
         <v>1</v>
       </c>
@@ -8669,7 +8673,7 @@
         <v>1035.5</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="20">
         <v>1</v>
       </c>
@@ -8701,7 +8705,7 @@
         <v>1031.3</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="20">
         <v>1</v>
       </c>
@@ -8736,7 +8740,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="20">
         <v>1</v>
       </c>
@@ -8768,7 +8772,7 @@
         <v>1045.9000000000001</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="20">
         <v>1</v>
       </c>
@@ -8800,7 +8804,7 @@
         <v>1062.7</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="20">
         <v>1</v>
       </c>
@@ -8832,7 +8836,7 @@
         <v>1052.3</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="20">
         <v>1</v>
       </c>
@@ -8864,7 +8868,7 @@
         <v>1042.3</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="20">
         <v>1</v>
       </c>
@@ -8896,7 +8900,7 @@
         <v>1033.5999999999999</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="20">
         <v>1</v>
       </c>
@@ -8931,7 +8935,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="20">
         <v>1</v>
       </c>
@@ -8963,7 +8967,7 @@
         <v>1025.7</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="20">
         <v>1</v>
       </c>
@@ -8995,7 +8999,7 @@
         <v>1051.5999999999999</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="20">
         <v>1</v>
       </c>
@@ -9030,7 +9034,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="20">
         <v>1</v>
       </c>
@@ -9065,7 +9069,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="20">
         <v>1</v>
       </c>
@@ -9100,7 +9104,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="20">
         <v>1</v>
       </c>
@@ -9132,7 +9136,7 @@
         <v>1020.7</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="20">
         <v>1</v>
       </c>
@@ -9164,7 +9168,7 @@
         <v>1034.9000000000001</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="20">
         <v>1</v>
       </c>
@@ -9196,7 +9200,7 @@
         <v>1054.5999999999999</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="20">
         <v>1</v>
       </c>
@@ -9219,7 +9223,7 @@
         <v>1073.5999999999999</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="20">
         <v>1</v>
       </c>
@@ -9251,7 +9255,7 @@
         <v>1035.4000000000001</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="20">
         <v>1</v>
       </c>
@@ -9286,7 +9290,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="20">
         <v>1</v>
       </c>
@@ -9318,7 +9322,7 @@
         <v>1077.2</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="20">
         <v>1</v>
       </c>
@@ -9350,7 +9354,7 @@
         <v>1045.7</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="20">
         <v>1</v>
       </c>
@@ -9382,7 +9386,7 @@
         <v>1062.5</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="20">
         <v>1</v>
       </c>
@@ -9414,7 +9418,7 @@
         <v>1052.0999999999999</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="20">
         <v>1</v>
       </c>
@@ -9446,7 +9450,7 @@
         <v>1042.2</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="20">
         <v>1</v>
       </c>
@@ -9478,7 +9482,7 @@
         <v>1033.4000000000001</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="20">
         <v>1</v>
       </c>
@@ -9510,7 +9514,7 @@
         <v>1034.7</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="20">
         <v>1</v>
       </c>
@@ -9542,7 +9546,7 @@
         <v>1025.5</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="20">
         <v>1</v>
       </c>
@@ -9577,7 +9581,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="20">
         <v>1</v>
       </c>
@@ -9609,7 +9613,7 @@
         <v>1053.5</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" s="20">
         <v>1</v>
       </c>
@@ -9641,7 +9645,7 @@
         <v>1031.4000000000001</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="20">
         <v>1</v>
       </c>
@@ -9673,7 +9677,7 @@
         <v>1047.3</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" s="20">
         <v>1</v>
       </c>
@@ -9705,7 +9709,7 @@
         <v>1020.5</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="20">
         <v>1</v>
       </c>
@@ -9737,7 +9741,7 @@
         <v>1034.7</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="20">
         <v>1</v>
       </c>
@@ -9769,7 +9773,7 @@
         <v>1054.4000000000001</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="20">
         <v>1</v>
       </c>
@@ -9798,7 +9802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="20">
         <v>2</v>
       </c>
@@ -9833,7 +9837,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="20">
         <v>2</v>
       </c>
@@ -9865,7 +9869,7 @@
         <v>989.9</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="20">
         <v>2</v>
       </c>
@@ -9897,7 +9901,7 @@
         <v>986.5</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="20">
         <v>2</v>
       </c>
@@ -9929,7 +9933,7 @@
         <v>826.2</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="20">
         <v>2</v>
       </c>
@@ -9961,7 +9965,7 @@
         <v>842.7</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="20">
         <v>2</v>
       </c>
@@ -9993,7 +9997,7 @@
         <v>839.3</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="20">
         <v>2</v>
       </c>
@@ -10025,7 +10029,7 @@
         <v>845.4</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="20">
         <v>2</v>
       </c>
@@ -10057,7 +10061,7 @@
         <v>853.2</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="20">
         <v>2</v>
       </c>
@@ -10089,7 +10093,7 @@
         <v>847.9</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" s="20">
         <v>2</v>
       </c>
@@ -10121,7 +10125,7 @@
         <v>1037.8</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" s="20">
         <v>2</v>
       </c>
@@ -10153,7 +10157,7 @@
         <v>1022.1</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" s="20">
         <v>2</v>
       </c>
@@ -10185,7 +10189,7 @@
         <v>1049.3</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" s="20">
         <v>2</v>
       </c>
@@ -10217,7 +10221,7 @@
         <v>951.5</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" s="20">
         <v>2</v>
       </c>
@@ -10249,7 +10253,7 @@
         <v>858</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" s="20">
         <v>2</v>
       </c>
@@ -10281,7 +10285,7 @@
         <v>847.3</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" s="20">
         <v>2</v>
       </c>
@@ -10313,7 +10317,7 @@
         <v>838.3</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" s="20">
         <v>2</v>
       </c>
@@ -10345,7 +10349,7 @@
         <v>852.1</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" s="20">
         <v>2</v>
       </c>
@@ -10377,7 +10381,7 @@
         <v>863.3</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" s="20">
         <v>2</v>
       </c>
@@ -10409,7 +10413,7 @@
         <v>851.1</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" s="20">
         <v>2</v>
       </c>
@@ -10441,7 +10445,7 @@
         <v>841.2</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" s="20">
         <v>2</v>
       </c>
@@ -10473,7 +10477,7 @@
         <v>871.6</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" s="20">
         <v>2</v>
       </c>
@@ -10505,7 +10509,7 @@
         <v>826.9</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" s="20">
         <v>2</v>
       </c>
@@ -10537,7 +10541,7 @@
         <v>1073.5999999999999</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" s="20">
         <v>2</v>
       </c>
@@ -10560,7 +10564,7 @@
         <v>826.9</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" s="20">
         <v>2</v>
       </c>
@@ -10595,7 +10599,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" s="20">
         <v>2</v>
       </c>
@@ -10627,7 +10631,7 @@
         <v>857.2</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" s="20">
         <v>2</v>
       </c>
@@ -10650,7 +10654,7 @@
         <v>1073.5999999999999</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" s="20">
         <v>2</v>
       </c>
@@ -10685,7 +10689,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" s="20">
         <v>2</v>
       </c>
@@ -10717,7 +10721,7 @@
         <v>850.9</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" s="20">
         <v>2</v>
       </c>
@@ -10749,7 +10753,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" s="20">
         <v>2</v>
       </c>
@@ -10781,7 +10785,7 @@
         <v>871.3</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" s="20">
         <v>2</v>
       </c>
@@ -10813,7 +10817,7 @@
         <v>1037</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" s="20">
         <v>2</v>
       </c>
@@ -10845,7 +10849,7 @@
         <v>1021.3</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" s="20">
         <v>2</v>
       </c>
@@ -10877,7 +10881,7 @@
         <v>1048.5999999999999</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" s="20">
         <v>2</v>
       </c>
@@ -10909,7 +10913,7 @@
         <v>844.2</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" s="20">
         <v>2</v>
       </c>
@@ -10941,7 +10945,7 @@
         <v>852.1</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" s="20">
         <v>2</v>
       </c>
@@ -10973,7 +10977,7 @@
         <v>846.9</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" s="20">
         <v>2</v>
       </c>
@@ -11005,7 +11009,7 @@
         <v>825.3</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" s="20">
         <v>2</v>
       </c>
@@ -11037,7 +11041,7 @@
         <v>841.8</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" s="20">
         <v>2</v>
       </c>
@@ -11069,7 +11073,7 @@
         <v>838.5</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" s="20">
         <v>2</v>
       </c>
@@ -11101,7 +11105,7 @@
         <v>959.8</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" s="20">
         <v>2</v>
       </c>
@@ -11133,7 +11137,7 @@
         <v>989.8</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" s="20">
         <v>2</v>
       </c>
@@ -11165,7 +11169,7 @@
         <v>986.4</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" s="20">
         <v>2</v>
       </c>
@@ -11197,7 +11201,7 @@
         <v>838.2</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" s="20">
         <v>2</v>
       </c>
@@ -11229,7 +11233,7 @@
         <v>851.9</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" s="20">
         <v>2</v>
       </c>
@@ -11261,7 +11265,7 @@
         <v>863.2</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" s="20">
         <v>2</v>
       </c>
@@ -11284,7 +11288,7 @@
         <v>1073.5999999999999</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" s="20">
         <v>2</v>
       </c>
@@ -11316,7 +11320,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" s="20">
         <v>2</v>
       </c>
@@ -11348,7 +11352,7 @@
         <v>851.8</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" s="20">
         <v>2</v>
       </c>
@@ -11380,7 +11384,7 @@
         <v>863.1</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" s="20">
         <v>2</v>
       </c>
@@ -11412,7 +11416,7 @@
         <v>824.3</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" s="20">
         <v>2</v>
       </c>
@@ -11444,7 +11448,7 @@
         <v>840.8</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" s="20">
         <v>2</v>
       </c>
@@ -11476,7 +11480,7 @@
         <v>837.5</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" s="20">
         <v>2</v>
       </c>
@@ -11499,7 +11503,7 @@
         <v>405.96</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" s="20">
         <v>2</v>
       </c>
@@ -11522,7 +11526,7 @@
         <v>826.9</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" s="20">
         <v>2</v>
       </c>
@@ -11554,7 +11558,7 @@
         <v>959.7</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" s="20">
         <v>2</v>
       </c>
@@ -11586,7 +11590,7 @@
         <v>989.7</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" s="20">
         <v>2</v>
       </c>
@@ -11621,7 +11625,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" s="20">
         <v>2</v>
       </c>
@@ -11653,7 +11657,7 @@
         <v>1036.4000000000001</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" s="20">
         <v>2</v>
       </c>
@@ -11685,7 +11689,7 @@
         <v>1020.6</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" s="20">
         <v>2</v>
       </c>
@@ -11717,7 +11721,7 @@
         <v>1048</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" s="20">
         <v>2</v>
       </c>
@@ -11749,7 +11753,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" s="20">
         <v>2</v>
       </c>
@@ -11781,7 +11785,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" s="20">
         <v>2</v>
       </c>
@@ -11813,7 +11817,7 @@
         <v>845.7</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" s="20">
         <v>2</v>
       </c>
@@ -11845,7 +11849,7 @@
         <v>949.3</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" s="20">
         <v>2</v>
       </c>
@@ -11877,7 +11881,7 @@
         <v>856.4</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" s="20">
         <v>2</v>
       </c>
@@ -11909,7 +11913,7 @@
         <v>845.8</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" s="20">
         <v>2</v>
       </c>
@@ -11941,7 +11945,7 @@
         <v>850.6</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" s="20">
         <v>2</v>
       </c>
@@ -11973,7 +11977,7 @@
         <v>840.8</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" s="20">
         <v>2</v>
       </c>
@@ -12005,7 +12009,7 @@
         <v>871.1</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" s="20">
         <v>2</v>
       </c>
@@ -12037,7 +12041,7 @@
         <v>948.5</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" s="20">
         <v>2</v>
       </c>
@@ -12069,7 +12073,7 @@
         <v>855.7</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" s="20">
         <v>2</v>
       </c>
@@ -12101,7 +12105,7 @@
         <v>845.2</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" s="20">
         <v>2</v>
       </c>
@@ -12133,7 +12137,7 @@
         <v>849.8</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" s="20">
         <v>2</v>
       </c>
@@ -12165,7 +12169,7 @@
         <v>839.9</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" s="20">
         <v>2</v>
       </c>
@@ -12197,7 +12201,7 @@
         <v>870.2</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" s="20">
         <v>2</v>
       </c>
@@ -12229,7 +12233,7 @@
         <v>1035.8</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" s="20">
         <v>2</v>
       </c>
@@ -12261,7 +12265,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" s="20">
         <v>2</v>
       </c>
@@ -12293,7 +12297,7 @@
         <v>1047.5</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" s="20">
         <v>2</v>
       </c>
@@ -12325,7 +12329,7 @@
         <v>842.4</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" s="20">
         <v>2</v>
       </c>
@@ -12357,7 +12361,7 @@
         <v>850.5</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" s="20">
         <v>2</v>
       </c>
@@ -12389,7 +12393,7 @@
         <v>845.3</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" s="20">
         <v>2</v>
       </c>
@@ -12421,7 +12425,7 @@
         <v>823.8</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" s="20">
         <v>2</v>
       </c>
@@ -12453,7 +12457,7 @@
         <v>840.3</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" s="20">
         <v>2</v>
       </c>
@@ -12485,7 +12489,7 @@
         <v>837.1</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" s="20">
         <v>2</v>
       </c>
@@ -12520,7 +12524,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" s="20">
         <v>2</v>
       </c>
@@ -12552,7 +12556,7 @@
         <v>989.6</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" s="20">
         <v>2</v>
       </c>
@@ -12584,7 +12588,7 @@
         <v>986.2</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" s="20">
         <v>2</v>
       </c>
@@ -12616,7 +12620,7 @@
         <v>837.4</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" s="20">
         <v>2</v>
       </c>
@@ -12648,7 +12652,7 @@
         <v>851.3</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" s="20">
         <v>2</v>
       </c>
@@ -12680,7 +12684,7 @@
         <v>862.4</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" s="20">
         <v>2</v>
       </c>
@@ -12706,7 +12710,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" s="20">
         <v>2</v>
       </c>
@@ -12732,7 +12736,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" s="20">
         <v>2</v>
       </c>
@@ -12758,7 +12762,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" s="20">
         <v>2</v>
       </c>
@@ -12790,7 +12794,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" s="20">
         <v>2</v>
       </c>
@@ -12822,7 +12826,7 @@
         <v>850.9</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" s="20">
         <v>2</v>
       </c>
@@ -12854,7 +12858,7 @@
         <v>861.9</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" s="20">
         <v>2</v>
       </c>
@@ -12886,7 +12890,7 @@
         <v>823.5</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" s="20">
         <v>2</v>
       </c>
@@ -12918,7 +12922,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" s="20">
         <v>2</v>
       </c>
@@ -12950,7 +12954,7 @@
         <v>836.8</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" s="20">
         <v>2</v>
       </c>
@@ -12982,7 +12986,7 @@
         <v>959.6</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" s="20">
         <v>2</v>
       </c>
@@ -13014,7 +13018,7 @@
         <v>989.6</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" s="20">
         <v>2</v>
       </c>
@@ -13046,7 +13050,7 @@
         <v>986.1</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" s="20">
         <v>2</v>
       </c>
@@ -13078,7 +13082,7 @@
         <v>1035.4000000000001</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" s="20">
         <v>2</v>
       </c>
@@ -13110,7 +13114,7 @@
         <v>1019.5</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" s="20">
         <v>2</v>
       </c>
@@ -13142,7 +13146,7 @@
         <v>1047.0999999999999</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290" s="20">
         <v>2</v>
       </c>
@@ -13174,7 +13178,7 @@
         <v>842.1</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291" s="20">
         <v>2</v>
       </c>
@@ -13206,7 +13210,7 @@
         <v>850.3</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292" s="20">
         <v>2</v>
       </c>
@@ -13238,7 +13242,7 @@
         <v>845.1</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293" s="20">
         <v>2</v>
       </c>
@@ -13270,7 +13274,7 @@
         <v>947.9</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294" s="20">
         <v>2</v>
       </c>
@@ -13302,7 +13306,7 @@
         <v>855.1</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295" s="20">
         <v>2</v>
       </c>
@@ -13334,7 +13338,7 @@
         <v>844.8</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296" s="20">
         <v>2</v>
       </c>
@@ -13366,7 +13370,7 @@
         <v>849.5</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297" s="20">
         <v>2</v>
       </c>
@@ -13398,7 +13402,7 @@
         <v>839.6</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A298" s="20">
         <v>2</v>
       </c>
@@ -13430,7 +13434,7 @@
         <v>869.8</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A299" s="20">
         <v>2</v>
       </c>
@@ -13453,7 +13457,7 @@
         <v>826.9</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A300" s="20">
         <v>2</v>
       </c>
@@ -13476,7 +13480,7 @@
         <v>405.97</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301" s="20">
         <v>2</v>
       </c>
@@ -13499,7 +13503,7 @@
         <v>1073.5999999999999</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302" s="20">
         <v>2</v>
       </c>
@@ -13531,7 +13535,7 @@
         <v>849.3</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A303" s="20">
         <v>2</v>
       </c>
@@ -13563,7 +13567,7 @@
         <v>839.5</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304" s="20">
         <v>2</v>
       </c>
@@ -13595,7 +13599,7 @@
         <v>869.7</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305" s="20">
         <v>2</v>
       </c>
@@ -13627,7 +13631,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A306" s="20">
         <v>2</v>
       </c>
@@ -13659,7 +13663,7 @@
         <v>850.1</v>
       </c>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A307" s="20">
         <v>2</v>
       </c>
@@ -13691,7 +13695,7 @@
         <v>844.9</v>
       </c>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A308" s="20">
         <v>2</v>
       </c>
@@ -13723,7 +13727,7 @@
         <v>947.6</v>
       </c>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A309" s="20">
         <v>2</v>
       </c>
@@ -13755,7 +13759,7 @@
         <v>854.8</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A310" s="20">
         <v>2</v>
       </c>
@@ -13787,7 +13791,7 @@
         <v>844.5</v>
       </c>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A311" s="20">
         <v>2</v>
       </c>
@@ -13819,7 +13823,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A312" s="20">
         <v>2</v>
       </c>
@@ -13851,7 +13855,7 @@
         <v>1019.2</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313" s="20">
         <v>2</v>
       </c>
@@ -13886,7 +13890,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314" s="20">
         <v>2</v>
       </c>
@@ -13918,7 +13922,7 @@
         <v>823.2</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315" s="20">
         <v>2</v>
       </c>
@@ -13953,7 +13957,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A316" s="20">
         <v>2</v>
       </c>
@@ -13985,7 +13989,7 @@
         <v>836.6</v>
       </c>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A317" s="20">
         <v>2</v>
       </c>
@@ -14017,7 +14021,7 @@
         <v>959.5</v>
       </c>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A318" s="20">
         <v>2</v>
       </c>
@@ -14049,7 +14053,7 @@
         <v>989.5</v>
       </c>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A319" s="20">
         <v>2</v>
       </c>
@@ -14081,7 +14085,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320" s="20">
         <v>2</v>
       </c>
@@ -14113,7 +14117,7 @@
         <v>836.8</v>
       </c>
     </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A321" s="20">
         <v>2</v>
       </c>
@@ -14145,7 +14149,7 @@
         <v>850.6</v>
       </c>
     </row>
-    <row r="322" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A322" s="20">
         <v>2</v>
       </c>
@@ -14177,7 +14181,7 @@
         <v>861.6</v>
       </c>
     </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A323" s="20">
         <v>2</v>
       </c>
@@ -14200,7 +14204,7 @@
         <v>826.9</v>
       </c>
     </row>
-    <row r="324" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A324" s="20">
         <v>2</v>
       </c>
@@ -14223,7 +14227,7 @@
         <v>1073.5999999999999</v>
       </c>
     </row>
-    <row r="325" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A325" s="20">
         <v>2</v>
       </c>
@@ -14246,7 +14250,7 @@
         <v>405.96</v>
       </c>
     </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A326" s="20">
         <v>2</v>
       </c>
@@ -14281,7 +14285,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="327" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A327" s="20">
         <v>2</v>
       </c>
@@ -14313,7 +14317,7 @@
         <v>850.4</v>
       </c>
     </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A328" s="20">
         <v>2</v>
       </c>
@@ -14345,7 +14349,7 @@
         <v>861.4</v>
       </c>
     </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A329" s="20">
         <v>2</v>
       </c>
@@ -14377,7 +14381,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="330" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A330" s="20">
         <v>2</v>
       </c>
@@ -14409,7 +14413,7 @@
         <v>839.5</v>
       </c>
     </row>
-    <row r="331" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A331" s="20">
         <v>2</v>
       </c>
@@ -14441,7 +14445,7 @@
         <v>836.4</v>
       </c>
     </row>
-    <row r="332" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A332" s="20">
         <v>2</v>
       </c>
@@ -14473,7 +14477,7 @@
         <v>959.3</v>
       </c>
     </row>
-    <row r="333" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A333" s="20">
         <v>2</v>
       </c>
@@ -14505,7 +14509,7 @@
         <v>989.3</v>
       </c>
     </row>
-    <row r="334" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A334" s="20">
         <v>2</v>
       </c>
@@ -14537,7 +14541,7 @@
         <v>985.9</v>
       </c>
     </row>
-    <row r="335" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A335" s="20">
         <v>2</v>
       </c>
@@ -14569,7 +14573,7 @@
         <v>841.8</v>
       </c>
     </row>
-    <row r="336" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A336" s="20">
         <v>2</v>
       </c>
@@ -14601,7 +14605,7 @@
         <v>849.9</v>
       </c>
     </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A337" s="20">
         <v>2</v>
       </c>
@@ -14633,7 +14637,7 @@
         <v>844.7</v>
       </c>
     </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A338" s="20">
         <v>2</v>
       </c>
@@ -14665,7 +14669,7 @@
         <v>1034.7</v>
       </c>
     </row>
-    <row r="339" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A339" s="20">
         <v>2</v>
       </c>
@@ -14700,7 +14704,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A340" s="20">
         <v>2</v>
       </c>
@@ -14732,7 +14736,7 @@
         <v>1046.5</v>
       </c>
     </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A341" s="20">
         <v>2</v>
       </c>
@@ -14764,7 +14768,7 @@
         <v>849.2</v>
       </c>
     </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A342" s="20">
         <v>2</v>
       </c>
@@ -14796,7 +14800,7 @@
         <v>839.4</v>
       </c>
     </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A343" s="20">
         <v>2</v>
       </c>
@@ -14831,7 +14835,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A344" s="20">
         <v>2</v>
       </c>
@@ -14863,7 +14867,7 @@
         <v>947.2</v>
       </c>
     </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A345" s="20">
         <v>2</v>
       </c>
@@ -14898,7 +14902,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A346" s="20">
         <v>2</v>
       </c>
@@ -14930,7 +14934,7 @@
         <v>844.2</v>
       </c>
     </row>
-    <row r="347" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A347" s="20">
         <v>2</v>
       </c>
@@ -14950,7 +14954,7 @@
         <v>1073.5999999999999</v>
       </c>
     </row>
-    <row r="348" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A348" s="20">
         <v>2</v>
       </c>
@@ -14970,7 +14974,7 @@
         <v>826.9</v>
       </c>
     </row>
-    <row r="349" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A349" s="20">
         <v>2</v>
       </c>
@@ -14990,7 +14994,7 @@
         <v>405.96</v>
       </c>
     </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A350" s="20">
         <v>2</v>
       </c>
@@ -15022,7 +15026,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A351" s="20">
         <v>2</v>
       </c>
@@ -15054,7 +15058,7 @@
         <v>854.4</v>
       </c>
     </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A352" s="20">
         <v>2</v>
       </c>
@@ -15100,7 +15104,7 @@
         <v>1010</v>
       </c>
       <c r="E353" s="20">
-        <v>1010</v>
+        <v>1013</v>
       </c>
       <c r="F353" s="20">
         <v>352</v>
@@ -15722,7 +15726,7 @@
         <v>405.94</v>
       </c>
     </row>
-    <row r="374" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A374" s="20">
         <v>2</v>
       </c>
@@ -15754,7 +15758,7 @@
         <v>946.8</v>
       </c>
     </row>
-    <row r="375" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A375" s="20">
         <v>2</v>
       </c>
@@ -15786,7 +15790,7 @@
         <v>854.2</v>
       </c>
     </row>
-    <row r="376" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A376" s="20">
         <v>2</v>
       </c>
@@ -15818,7 +15822,7 @@
         <v>843.9</v>
       </c>
     </row>
-    <row r="377" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A377" s="20">
         <v>2</v>
       </c>
@@ -15850,7 +15854,7 @@
         <v>1034.4000000000001</v>
       </c>
     </row>
-    <row r="378" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A378" s="20">
         <v>2</v>
       </c>
@@ -15882,7 +15886,7 @@
         <v>1018.5</v>
       </c>
     </row>
-    <row r="379" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A379" s="20">
         <v>2</v>
       </c>
@@ -15914,7 +15918,7 @@
         <v>1046.2</v>
       </c>
     </row>
-    <row r="380" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A380" s="20">
         <v>2</v>
       </c>
@@ -15946,7 +15950,7 @@
         <v>959.2</v>
       </c>
     </row>
-    <row r="381" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A381" s="20">
         <v>2</v>
       </c>
@@ -15978,7 +15982,7 @@
         <v>989.1</v>
       </c>
     </row>
-    <row r="382" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A382" s="20">
         <v>2</v>
       </c>
@@ -16010,7 +16014,7 @@
         <v>985.7</v>
       </c>
     </row>
-    <row r="383" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A383" s="20">
         <v>2</v>
       </c>
@@ -16042,7 +16046,7 @@
         <v>849.1</v>
       </c>
     </row>
-    <row r="384" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A384" s="20">
         <v>2</v>
       </c>
@@ -16074,7 +16078,7 @@
         <v>839.2</v>
       </c>
     </row>
-    <row r="385" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A385" s="20">
         <v>2</v>
       </c>
@@ -16106,7 +16110,7 @@
         <v>869.4</v>
       </c>
     </row>
-    <row r="386" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A386" s="20">
         <v>2</v>
       </c>
@@ -16138,7 +16142,7 @@
         <v>841.5</v>
       </c>
     </row>
-    <row r="387" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A387" s="20">
         <v>2</v>
       </c>
@@ -16170,7 +16174,7 @@
         <v>849.7</v>
       </c>
     </row>
-    <row r="388" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A388" s="20">
         <v>2</v>
       </c>
@@ -16202,7 +16206,7 @@
         <v>844.5</v>
       </c>
     </row>
-    <row r="389" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A389" s="20">
         <v>2</v>
       </c>
@@ -16234,7 +16238,7 @@
         <v>836.4</v>
       </c>
     </row>
-    <row r="390" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A390" s="20">
         <v>2</v>
       </c>
@@ -16266,7 +16270,7 @@
         <v>850.2</v>
       </c>
     </row>
-    <row r="391" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A391" s="20">
         <v>2</v>
       </c>
@@ -16298,7 +16302,7 @@
         <v>861.2</v>
       </c>
     </row>
-    <row r="392" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A392" s="20">
         <v>2</v>
       </c>
@@ -16330,7 +16334,7 @@
         <v>822.8</v>
       </c>
     </row>
-    <row r="393" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A393" s="20">
         <v>2</v>
       </c>
@@ -16365,7 +16369,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="394" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A394" s="20">
         <v>2</v>
       </c>
@@ -16397,7 +16401,7 @@
         <v>836.2</v>
       </c>
     </row>
-    <row r="395" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A395" s="20">
         <v>2</v>
       </c>
@@ -16417,7 +16421,7 @@
         <v>1073.5999999999999</v>
       </c>
     </row>
-    <row r="396" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A396" s="20">
         <v>2</v>
       </c>
@@ -16437,7 +16441,7 @@
         <v>826.9</v>
       </c>
     </row>
-    <row r="397" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A397" s="20">
         <v>2</v>
       </c>
@@ -16457,7 +16461,7 @@
         <v>405.95</v>
       </c>
     </row>
-    <row r="398" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A398" s="20">
         <v>2</v>
       </c>
@@ -16492,7 +16496,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="399" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A399" s="20">
         <v>2</v>
       </c>
@@ -16524,7 +16528,7 @@
         <v>839.1</v>
       </c>
     </row>
-    <row r="400" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A400" s="20">
         <v>2</v>
       </c>
@@ -16556,7 +16560,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="401" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A401" s="20">
         <v>2</v>
       </c>
@@ -16588,7 +16592,7 @@
         <v>841.4</v>
       </c>
     </row>
-    <row r="402" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A402" s="20">
         <v>2</v>
       </c>
@@ -16620,7 +16624,7 @@
         <v>849.5</v>
       </c>
     </row>
-    <row r="403" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A403" s="20">
         <v>2</v>
       </c>
@@ -16652,7 +16656,7 @@
         <v>844.3</v>
       </c>
     </row>
-    <row r="404" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A404" s="20">
         <v>2</v>
       </c>
@@ -16684,7 +16688,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="405" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A405" s="20">
         <v>2</v>
       </c>
@@ -16716,7 +16720,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="406" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A406" s="20">
         <v>2</v>
       </c>
@@ -16748,7 +16752,7 @@
         <v>985.5</v>
       </c>
     </row>
-    <row r="407" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A407" s="20">
         <v>2</v>
       </c>
@@ -16780,7 +16784,7 @@
         <v>946.5</v>
       </c>
     </row>
-    <row r="408" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A408" s="20">
         <v>2</v>
       </c>
@@ -16815,7 +16819,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="409" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A409" s="20">
         <v>2</v>
       </c>
@@ -16850,7 +16854,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="410" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A410" s="20">
         <v>2</v>
       </c>
@@ -16882,7 +16886,7 @@
         <v>836.2</v>
       </c>
     </row>
-    <row r="411" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A411" s="20">
         <v>2</v>
       </c>
@@ -16914,7 +16918,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="412" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A412" s="20">
         <v>2</v>
       </c>
@@ -16946,7 +16950,7 @@
         <v>861</v>
       </c>
     </row>
-    <row r="413" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A413" s="20">
         <v>2</v>
       </c>
@@ -16978,7 +16982,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="414" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A414" s="20">
         <v>2</v>
       </c>
@@ -17010,7 +17014,7 @@
         <v>839.1</v>
       </c>
     </row>
-    <row r="415" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A415" s="20">
         <v>2</v>
       </c>
@@ -17042,7 +17046,7 @@
         <v>869.3</v>
       </c>
     </row>
-    <row r="416" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A416" s="20">
         <v>2</v>
       </c>
@@ -17077,7 +17081,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="417" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A417" s="20">
         <v>2</v>
       </c>
@@ -17109,7 +17113,7 @@
         <v>1018.3</v>
       </c>
     </row>
-    <row r="418" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A418" s="20">
         <v>2</v>
       </c>
@@ -17144,7 +17148,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="419" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A419" s="20">
         <v>2</v>
       </c>
@@ -17164,7 +17168,7 @@
         <v>1073.5999999999999</v>
       </c>
     </row>
-    <row r="420" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A420" s="20">
         <v>2</v>
       </c>
@@ -17184,7 +17188,7 @@
         <v>826.9</v>
       </c>
     </row>
-    <row r="421" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A421" s="20">
         <v>2</v>
       </c>
@@ -17205,6 +17209,19 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K421">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="2"/>
+        <filter val="exper"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="1022017"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -17213,7 +17230,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" workbookViewId="0">
+    <sheetView windowProtection="1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>